<commit_message>
Ditto Pachen - for Aug release
</commit_message>
<xml_diff>
--- a/Development/Artifacts/Changes From 28 May.xlsx
+++ b/Development/Artifacts/Changes From 28 May.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
     <t>Bugzilla Ticket No</t>
   </si>
@@ -58,6 +58,38 @@
   </si>
   <si>
     <t>Need to do builds as class file and UIM is changed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The database field type has been changed to CLOB for IDTABBEDLIST as the bulk sms was not working for more than 500 
+ALTER TABLE MOLSASMSWMINSTANCE ADD IDTABBEDLIST1 CLOB;
+update MOLSASMSWMINSTANCE set IDTABBEDLIST1=IDTABBEDLIST;
+ALTER TABLE MOLSASMSWMINSTANCE drop column IDTABBEDLIST ;
+ALTER TABLE MOLSASMSWMINSTANCE rename column  IDTABBEDLIST1 to IDTABBEDLIST;
+</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Ditto</t>
+  </si>
+  <si>
+    <t>New ear and SQL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The database field type has been changed to CLOB for IDTABBEDLIST as the bulk sms was not working for more than 500 </t>
+  </si>
+  <si>
+    <t>Test the bulk sms</t>
+  </si>
+  <si>
+    <t>ALTER TABLE MOLSAInformationRequest  ADD createdByvarchar2(64);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IP   Request is not saving the details of who created it </t>
+  </si>
+  <si>
+    <t>Test the IP Request Page</t>
   </si>
 </sst>
 </file>
@@ -122,7 +154,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -136,9 +168,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -447,9 +476,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -517,15 +546,51 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
+    <row r="4" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>42236</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="C5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="I5" s="1"/>
+      <c r="A5" s="2">
+        <v>42236</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C6" s="6"/>
@@ -609,6 +674,34 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="e967487d-3eea-483d-b969-e50e6c114ffa">UQKZYU5EZKJQ-17-950</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="e967487d-3eea-483d-b969-e50e6c114ffa">
+      <Url>https://dionatec.sharepoint.com/GlobalServices/_layouts/15/DocIdRedir.aspx?ID=UQKZYU5EZKJQ-17-950</Url>
+      <Description>UQKZYU5EZKJQ-17-950</Description>
+    </_dlc_DocIdUrl>
+    <SharedWithUsers xmlns="e967487d-3eea-483d-b969-e50e6c114ffa">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003520CC91E1C90A4F9689A135D663C63F" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5bea9beecb72e899f05172e22af69af0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e967487d-3eea-483d-b969-e50e6c114ffa" xmlns:ns3="43475cab-d89f-451e-a1e3-4db005e0f558" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="438d5435a0413bb8242127eebe6f163c" ns2:_="" ns3:_="">
     <xsd:import namespace="e967487d-3eea-483d-b969-e50e6c114ffa"/>
@@ -792,34 +885,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocId xmlns="e967487d-3eea-483d-b969-e50e6c114ffa">UQKZYU5EZKJQ-17-950</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="e967487d-3eea-483d-b969-e50e6c114ffa">
-      <Url>https://dionatec.sharepoint.com/GlobalServices/_layouts/15/DocIdRedir.aspx?ID=UQKZYU5EZKJQ-17-950</Url>
-      <Description>UQKZYU5EZKJQ-17-950</Description>
-    </_dlc_DocIdUrl>
-    <SharedWithUsers xmlns="e967487d-3eea-483d-b969-e50e6c114ffa">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE6F0B25-6AD0-4AF9-AE4F-0D8285608470}">
   <ds:schemaRefs>
@@ -829,6 +894,31 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A3CD956-F256-4860-8B56-AE881D5ADEC8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1926F8BC-3749-487B-86BA-515B8CAD861D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="e967487d-3eea-483d-b969-e50e6c114ffa"/>
+    <ds:schemaRef ds:uri="43475cab-d89f-451e-a1e3-4db005e0f558"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F0051AA5-43D6-41A0-9086-D5D3DFF72221}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -845,29 +935,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1926F8BC-3749-487B-86BA-515B8CAD861D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="e967487d-3eea-483d-b969-e50e6c114ffa"/>
-    <ds:schemaRef ds:uri="43475cab-d89f-451e-a1e3-4db005e0f558"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A3CD956-F256-4860-8B56-AE881D5ADEC8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>